<commit_message>
now i have updated main file TO make attendance of STEP SCHOOL
</commit_message>
<xml_diff>
--- a/stud_data/STEP 2.xlsx
+++ b/stud_data/STEP 2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,106 @@
           <t>20-03-2025 Time</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>21-03-2025 Status</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>21-03-2025 Time</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>22-03-2025 Status</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>22-03-2025 Time</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>23-03-2025 Status</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>23-03-2025 Time</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>24-03-2025 Status</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>24-03-2025 Time</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>25-03-2025 Status</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>25-03-2025 Time</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>26-03-2025 Status</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>26-03-2025 Time</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>27-03-2025 Status</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>27-03-2025 Time</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>28-03-2025 Status</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>28-03-2025 Time</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>31-03-2025 Status</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>31-03-2025 Time</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>01-04-2025 Status</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>01-04-2025 Time</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -470,39 +570,223 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>13:48:30</t>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4202</v>
+        <v>4209</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ayat Eman</t>
+          <t>no one</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>13:48:35</t>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
         </is>
       </c>
     </row>
@@ -516,16 +800,108 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>13:48:26</t>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
         </is>
       </c>
     </row>
@@ -539,16 +915,108 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>13:48:21</t>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
         </is>
       </c>
     </row>
@@ -561,13 +1029,107 @@
           <t>Ameer Abbas</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
         <is>
           <t>00:00:00</t>
         </is>

</xml_diff>